<commit_message>
added code to run all models across multiple datasets and did some house cleaning
</commit_message>
<xml_diff>
--- a/datasets.xlsx
+++ b/datasets.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulo/GitRepos/learning_rate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBD5836-42B0-7E47-89F4-639898C10F99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508E1530-4F16-8C40-AAED-22CBE0DA076E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="460" windowWidth="22760" windowHeight="16640" xr2:uid="{08205A03-BE4A-7B44-A321-BE81925EDFFF}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="22760" windowHeight="16560" activeTab="1" xr2:uid="{08205A03-BE4A-7B44-A321-BE81925EDFFF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="list" sheetId="1" r:id="rId1"/>
+    <sheet name="check" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">check!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="73">
   <si>
     <t>StudentStep</t>
   </si>
@@ -74,9 +78,6 @@
     <t>LFA_AIC_Model0_v2</t>
   </si>
   <si>
-    <t>LFA_BIC_Model0</t>
-  </si>
-  <si>
     <t>new_supportType_topic</t>
   </si>
   <si>
@@ -143,9 +144,6 @@
     <t>Digital Games for Improving Number Sense</t>
   </si>
   <si>
-    <t>OLI Engineering Statics - Fall 2011 - CMU (74 students)</t>
-  </si>
-  <si>
     <t>Rau Fractions Dataset Fall 2011 (condition GF MIX)</t>
   </si>
   <si>
@@ -246,13 +244,25 @@
   </si>
   <si>
     <t>Dataset</t>
+  </si>
+  <si>
+    <t>itAFM</t>
+  </si>
+  <si>
+    <t>iAFM</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -278,13 +288,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -299,12 +327,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,11 +651,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A6561F-DB29-BB40-9507-E1A0D1B6ECD7}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -637,13 +669,13 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -663,18 +695,18 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f t="shared" ref="D2:D24" si="0">_xlfn.CONCAT("Opportunity (",B2,")")</f>
+        <f t="shared" ref="D2:D23" si="0">_xlfn.CONCAT("Opportunity (",B2,")")</f>
         <v>Opportunity (LFA_AIC_LIB_Model0)</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E23" si="1">_xlfn.CONCAT("KC (",B2,")")</f>
+        <f t="shared" ref="E2:E22" si="1">_xlfn.CONCAT("KC (",B2,")")</f>
         <v>KC (LFA_AIC_LIB_Model0)</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -685,7 +717,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -696,7 +728,7 @@
         <v>KC (Default2)</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -707,7 +739,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -718,7 +750,7 @@
         <v>KC (Response)</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -729,7 +761,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -740,7 +772,7 @@
         <v>KC (LFASearchAICWholeModel1)</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -751,7 +783,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -762,7 +794,7 @@
         <v>KC (Main-KC7-split)</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -773,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -784,7 +816,7 @@
         <v>KC (LFASearchModel1)</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -795,7 +827,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -806,7 +838,7 @@
         <v>KC (LFASearchAICWholeModel1)</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -817,7 +849,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -828,7 +860,7 @@
         <v>KC (Default_corrected)</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -839,7 +871,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -850,7 +882,7 @@
         <v>KC (Main-KC7-split_renamed-PVfixed-models)</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -861,7 +893,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -872,7 +904,7 @@
         <v>KC (KTskills-Mcontext-single-sep-ind-areas)</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -883,7 +915,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -894,7 +926,7 @@
         <v>KC (LFASearchAICWholeModel1)</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -905,7 +937,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -916,62 +948,62 @@
         <v>KC (LFA_AIC_Model0_v2)</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>1980</v>
+        <v>562</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Opportunity (LFA_BIC_Model0)</v>
+        <v>Opportunity (new_supportType_topic)</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>KC (LFA_BIC_Model0)</v>
+        <v>KC (new_supportType_topic)</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Opportunity (new_supportType_topic)</v>
+        <v>Opportunity (new_topic)</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>KC (new_supportType_topic)</v>
+        <v>KC (new_topic)</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -982,191 +1014,570 @@
         <v>KC (new_topic)</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Opportunity (new_topic)</v>
+        <v>Opportunity (Default_topic)</v>
       </c>
       <c r="E17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>KC (new_topic)</v>
+        <v>KC (Default_topic)</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Opportunity (Default_topic)</v>
+        <v>Opportunity (new_repr)</v>
       </c>
       <c r="E18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>KC (Default_topic)</v>
+        <v>KC (new_repr)</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Opportunity (new_repr)</v>
+        <v>Opportunity (Default_reprType_topic)</v>
       </c>
       <c r="E19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>KC (new_repr)</v>
+        <v>KC (Default_reprType_topic)</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>567</v>
+        <v>605</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Opportunity (Default_reprType_topic)</v>
+        <v>Opportunity (KTracedSkills-Concatenated)</v>
       </c>
       <c r="E20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>KC (Default_reprType_topic)</v>
+        <v>KC (KTracedSkills-Concatenated)</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>605</v>
+        <v>1935</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Opportunity (LFASearchBICModel1-PVfixed-models uploaded)</v>
+      </c>
+      <c r="E21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>KC (LFASearchBICModel1-PVfixed-models uploaded)</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="6" customFormat="1">
+      <c r="A22" s="5">
+        <v>1305</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Opportunity (KTracedSkills-Concatenated)</v>
-      </c>
-      <c r="E21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>KC (KTracedSkills-Concatenated)</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="D22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Opportunity (teaTitle)</v>
+      </c>
+      <c r="E22" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>KC (teaTitle)</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="2">
-        <v>1935</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="2" t="s">
+    <row r="23" spans="1:6" s="6" customFormat="1">
+      <c r="A23" s="5">
+        <v>1330</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Opportunity (LFASearchBICModel1-PVfixed-models uploaded)</v>
-      </c>
-      <c r="E22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>KC (LFASearchBICModel1-PVfixed-models uploaded)</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="D23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Opportunity (CCSS standard)</v>
+      </c>
+      <c r="E23" s="6" t="str">
+        <f t="shared" ref="E23" si="2">_xlfn.CONCAT("KC (",B23,")")</f>
+        <v>KC (CCSS standard)</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2">
-        <v>1305</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Opportunity (teaTitle)</v>
-      </c>
-      <c r="E23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>KC (teaTitle)</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="2">
-        <v>1330</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Opportunity (CCSS standard)</v>
-      </c>
-      <c r="E24" s="1" t="str">
-        <f t="shared" ref="E24" si="2">_xlfn.CONCAT("KC (",B24,")")</f>
-        <v>KC (CCSS standard)</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE076C4-E1A0-4F4E-95C3-1DCE123FF769}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="44.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
+        <v>99</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
+        <v>104</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1">
+      <c r="A4" s="2">
+        <v>115</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1">
+      <c r="A5" s="2">
+        <v>253</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
+        <v>271</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>308</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>1980</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>372</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
+        <v>1899</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
+        <v>392</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2">
+        <v>394</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
+        <v>445</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
+        <v>562</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
+        <v>563</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2">
+        <v>564</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>565</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="8" customFormat="1">
+      <c r="A18" s="2">
+        <v>566</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>567</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
+        <v>605</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="8" customFormat="1">
+      <c r="A21" s="2">
+        <v>1935</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2">
+        <v>1305</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2">
+        <v>1330</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{A4472E34-276B-8542-B4FA-A4168C94942D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
+      <sortCondition ref="A1:A23"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>